<commit_message>
Atualização atividade 01 - Quick Sort
</commit_message>
<xml_diff>
--- a/ativ-quick-sort-ed.xlsx
+++ b/ativ-quick-sort-ed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\Fatec\Outros semestres\ED - ZL\Exercicios\Resolvidos\algoritmos_ordenacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971A73D8-0CBA-4858-A1C1-DCE5B9A2D5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62225EC1-D79D-4F1E-8F2F-E59E6004946E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{52247291-3DD0-4D22-87C6-031CFEF1AC44}"/>
   </bookViews>
@@ -148,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -163,9 +163,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4432,7 +4429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D359864-7B65-4AC2-9B53-554E0297BEA8}">
   <dimension ref="A1:Z69"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="R61" sqref="R61"/>
     </sheetView>
   </sheetViews>
@@ -4444,12 +4441,12 @@
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B1" s="5"/>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
       <c r="H1" s="2">
         <v>74</v>
       </c>
@@ -4483,12 +4480,12 @@
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B2" s="4"/>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="H3" s="2">
@@ -4782,7 +4779,7 @@
       <c r="H30" s="4">
         <v>16</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="2">
         <v>20</v>
       </c>
       <c r="J30" s="2">
@@ -4814,7 +4811,7 @@
       <c r="H33" s="4">
         <v>16</v>
       </c>
-      <c r="I33" s="6">
+      <c r="I33" s="2">
         <v>20</v>
       </c>
       <c r="J33" s="2">
@@ -4846,7 +4843,7 @@
       <c r="H36" s="4">
         <v>16</v>
       </c>
-      <c r="I36" s="6">
+      <c r="I36" s="2">
         <v>20</v>
       </c>
       <c r="J36" s="2">
@@ -4878,7 +4875,7 @@
       <c r="H39" s="4">
         <v>16</v>
       </c>
-      <c r="I39" s="6">
+      <c r="I39" s="2">
         <v>20</v>
       </c>
       <c r="J39" s="2">
@@ -4910,7 +4907,7 @@
       <c r="H42" s="4">
         <v>16</v>
       </c>
-      <c r="I42" s="6">
+      <c r="I42" s="2">
         <v>20</v>
       </c>
       <c r="J42" s="2">
@@ -4942,7 +4939,7 @@
       <c r="H45" s="4">
         <v>16</v>
       </c>
-      <c r="I45" s="6">
+      <c r="I45" s="2">
         <v>20</v>
       </c>
       <c r="J45" s="2">
@@ -4974,7 +4971,7 @@
       <c r="H48" s="4">
         <v>16</v>
       </c>
-      <c r="I48" s="6">
+      <c r="I48" s="2">
         <v>20</v>
       </c>
       <c r="J48" s="4">
@@ -5006,7 +5003,7 @@
       <c r="H51" s="4">
         <v>16</v>
       </c>
-      <c r="I51" s="6">
+      <c r="I51" s="2">
         <v>20</v>
       </c>
       <c r="J51" s="4">
@@ -5038,7 +5035,7 @@
       <c r="H54" s="4">
         <v>16</v>
       </c>
-      <c r="I54" s="6">
+      <c r="I54" s="2">
         <v>20</v>
       </c>
       <c r="J54" s="4">
@@ -5056,7 +5053,7 @@
       <c r="N54" s="4">
         <v>74</v>
       </c>
-      <c r="O54" s="6">
+      <c r="O54" s="2">
         <v>58</v>
       </c>
       <c r="P54" s="3">
@@ -5070,7 +5067,7 @@
       <c r="H57" s="4">
         <v>16</v>
       </c>
-      <c r="I57" s="6">
+      <c r="I57" s="2">
         <v>20</v>
       </c>
       <c r="J57" s="4">
@@ -5088,7 +5085,7 @@
       <c r="N57" s="4">
         <v>74</v>
       </c>
-      <c r="O57" s="6">
+      <c r="O57" s="2">
         <v>58</v>
       </c>
       <c r="P57" s="3">
@@ -5102,7 +5099,7 @@
       <c r="H60" s="4">
         <v>16</v>
       </c>
-      <c r="I60" s="6">
+      <c r="I60" s="2">
         <v>20</v>
       </c>
       <c r="J60" s="4">
@@ -5120,7 +5117,7 @@
       <c r="N60" s="4">
         <v>74</v>
       </c>
-      <c r="O60" s="6">
+      <c r="O60" s="2">
         <v>58</v>
       </c>
       <c r="P60" s="3">
@@ -5134,7 +5131,7 @@
       <c r="H63" s="4">
         <v>16</v>
       </c>
-      <c r="I63" s="6">
+      <c r="I63" s="2">
         <v>20</v>
       </c>
       <c r="J63" s="4">
@@ -5166,7 +5163,7 @@
       <c r="H66" s="4">
         <v>16</v>
       </c>
-      <c r="I66" s="6">
+      <c r="I66" s="2">
         <v>20</v>
       </c>
       <c r="J66" s="4">
@@ -5241,7 +5238,7 @@
   <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5252,12 +5249,12 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" s="5"/>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
       <c r="H1" s="3">
         <v>44</v>
       </c>
@@ -5282,12 +5279,12 @@
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" s="4"/>
-      <c r="C2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="C2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="H4" s="3">
@@ -5523,7 +5520,7 @@
       <c r="H34" s="2">
         <v>38</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I34" s="2">
         <v>39</v>
       </c>
       <c r="J34" s="3">
@@ -5551,7 +5548,7 @@
       <c r="H37" s="2">
         <v>38</v>
       </c>
-      <c r="I37" s="6">
+      <c r="I37" s="2">
         <v>39</v>
       </c>
       <c r="J37" s="3">
@@ -5571,25 +5568,25 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="H40" s="9">
+      <c r="H40" s="8">
         <v>38</v>
       </c>
-      <c r="I40" s="8">
+      <c r="I40" s="7">
         <v>39</v>
       </c>
-      <c r="J40" s="8">
+      <c r="J40" s="7">
         <v>40</v>
       </c>
-      <c r="K40" s="8">
+      <c r="K40" s="7">
         <v>41</v>
       </c>
-      <c r="L40" s="8">
+      <c r="L40" s="7">
         <v>42</v>
       </c>
-      <c r="M40" s="7">
+      <c r="M40" s="6">
         <v>43</v>
       </c>
-      <c r="N40" s="7">
+      <c r="N40" s="6">
         <v>44</v>
       </c>
     </row>

</xml_diff>